<commit_message>
checkaccount api has been completed.
</commit_message>
<xml_diff>
--- a/Risk Analizi/360 Müşteri Riski Analiz Sistemi umut reply.xlsx
+++ b/Risk Analizi/360 Müşteri Riski Analiz Sistemi umut reply.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="344">
   <si>
     <t xml:space="preserve">Yazılım Logo</t>
   </si>
@@ -39,6 +39,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">H</t>
     </r>
@@ -48,6 +49,7 @@
         <color rgb="FF000000"/>
         <rFont val="Oşgeldin"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">oş geldin</t>
     </r>
@@ -114,7 +116,7 @@
     <t xml:space="preserve">FIRMA_ISMI</t>
   </si>
   <si>
-    <t xml:space="preserve">T.C.Kimlik Numarası</t>
+    <t xml:space="preserve">Mükellef Numarası</t>
   </si>
   <si>
     <t xml:space="preserve">big unsigned integer (13 byte)</t>
@@ -130,15 +132,6 @@
   </si>
   <si>
     <t xml:space="preserve">DOGUMYERI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vergi Numarası</t>
-  </si>
-  <si>
-    <t xml:space="preserve">? unsigned integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VERGINO</t>
   </si>
   <si>
     <t xml:space="preserve">Vergi Dairesi</t>
@@ -246,6 +239,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">a.</t>
     </r>
@@ -255,6 +249,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">     </t>
     </r>
@@ -264,6 +259,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Faaliyet Belgesi </t>
     </r>
@@ -284,6 +280,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">b.</t>
     </r>
@@ -293,6 +290,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">     </t>
     </r>
@@ -302,6 +300,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Vergi Beyannamesi</t>
     </r>
@@ -319,6 +318,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">c.</t>
     </r>
@@ -328,6 +328,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">     </t>
     </r>
@@ -337,6 +338,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">İmza Sirküleri</t>
     </r>
@@ -366,6 +368,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">b.</t>
     </r>
@@ -375,6 +378,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">     </t>
     </r>
@@ -384,6 +388,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Yönetim Kurulu yapısı</t>
     </r>
@@ -1211,6 +1216,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1232,6 +1238,7 @@
       <color rgb="FF000000"/>
       <name val="Oşgeldin"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1239,12 +1246,14 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1258,17 +1267,20 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="7"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1612,9 +1624,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1789200</xdr:colOff>
+      <xdr:colOff>1788840</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>24840</xdr:rowOff>
+      <xdr:rowOff>24480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1624,7 +1636,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1711800" y="2131560"/>
-          <a:ext cx="1586160" cy="1358280"/>
+          <a:ext cx="1585800" cy="1357920"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -1680,9 +1692,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1332000</xdr:colOff>
+      <xdr:colOff>1331640</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>50040</xdr:rowOff>
+      <xdr:rowOff>49680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1692,7 +1704,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3553560" y="2131560"/>
-          <a:ext cx="1623240" cy="1383480"/>
+          <a:ext cx="1622880" cy="1383120"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -1748,9 +1760,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>837360</xdr:colOff>
+      <xdr:colOff>837000</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>50040</xdr:rowOff>
+      <xdr:rowOff>49680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1760,7 +1772,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5394240" y="2131560"/>
-          <a:ext cx="1623960" cy="1383480"/>
+          <a:ext cx="1623600" cy="1383120"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -1816,9 +1828,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>265320</xdr:colOff>
+      <xdr:colOff>264960</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>37440</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1828,7 +1840,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7250400" y="2131560"/>
-          <a:ext cx="1532160" cy="1370880"/>
+          <a:ext cx="1531800" cy="1370520"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -1889,9 +1901,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3227040</xdr:colOff>
+      <xdr:colOff>3226680</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>11520</xdr:rowOff>
+      <xdr:rowOff>11160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1900,13 +1912,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
-        <a:srcRect l="1134" t="46778" r="66591" b="2896"/>
+        <a:srcRect l="1134" t="46778" r="66598" b="2896"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="465480" y="10227240"/>
-          <a:ext cx="3211560" cy="3440520"/>
+          <a:ext cx="3211200" cy="3440160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1927,9 +1939,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>468720</xdr:colOff>
+      <xdr:colOff>468360</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>150840</xdr:rowOff>
+      <xdr:rowOff>150480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1944,7 +1956,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3972240" y="10227240"/>
-          <a:ext cx="3293280" cy="3579840"/>
+          <a:ext cx="3292920" cy="3579480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1970,7 +1982,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.16"/>
@@ -2152,13 +2164,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="4.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51.33"/>
@@ -2249,40 +2261,43 @@
         <v>29</v>
       </c>
       <c r="D12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>21</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>21</v>
+      <c r="D15" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>37</v>
@@ -2307,79 +2322,79 @@
         <v>41</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>21</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>52</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="0" t="s">
         <v>55</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>56</v>
@@ -2387,46 +2402,47 @@
       <c r="E23" s="0" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="9" t="s">
+      <c r="F23" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="9" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="C25" s="11"/>
+      <c r="D25" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="E25" s="12" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="B26" s="11" t="s">
+      <c r="A26" s="10"/>
+      <c r="B26" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="12" t="s">
+      <c r="C26" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="D26" s="0" t="s">
         <v>64</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
       <c r="B27" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>67</v>
@@ -2441,213 +2457,200 @@
         <v>69</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D28" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="0" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10"/>
-      <c r="B29" s="13" t="s">
+      <c r="C29" s="11"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10"/>
+      <c r="B30" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" s="0" t="s">
+      <c r="C30" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C30" s="11"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="162.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="10"/>
       <c r="B31" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="162.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10"/>
       <c r="B32" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="B33" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E32" s="0" t="s">
+      <c r="C33" s="11"/>
+      <c r="D33" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10"/>
-      <c r="B33" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10" t="n">
-        <v>3</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>81</v>
-      </c>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="10"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10"/>
+      <c r="B36" s="15" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10"/>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="61.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B41" s="0" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
+      <c r="C41" s="16" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="7" t="s">
+      <c r="D41" s="14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="61.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="10" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="10" t="n">
-        <v>5</v>
-      </c>
-      <c r="B46" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="25.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="10"/>
+      <c r="B47" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="10"/>
+      <c r="C48" s="0" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="10" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="25.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="10"/>
-      <c r="B48" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="C48" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
-      <c r="J48" s="17"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="10"/>
-      <c r="C49" s="0" t="s">
-        <v>94</v>
+      <c r="B49" s="7" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="10"/>
-      <c r="B50" s="7" t="s">
-        <v>95</v>
+      <c r="A50" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="10" t="n">
         <v>2</v>
       </c>
     </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="C48:J48"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="C47:J47"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2670,7 +2673,7 @@
       <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="5.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.14"/>
@@ -2693,13 +2696,13 @@
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10"/>
       <c r="B2" s="0" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10"/>
       <c r="B3" s="0" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2711,28 +2714,28 @@
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10"/>
       <c r="D6" s="18" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="18" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19"/>
       <c r="B8" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="H8" s="0" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2740,17 +2743,17 @@
         <v>1</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="H9" s="0" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2758,18 +2761,18 @@
         <v>2</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
       <c r="H10" s="0" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>18</v>
@@ -2780,17 +2783,17 @@
         <v>3</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="H11" s="0" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2798,19 +2801,19 @@
         <v>4</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="H12" s="0" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2818,17 +2821,17 @@
         <v>5</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
       <c r="H13" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2836,28 +2839,28 @@
         <v>8</v>
       </c>
       <c r="B14" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="F14" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="H14" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="I14" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="J14" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2865,17 +2868,17 @@
         <v>6</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="H15" s="0" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2883,17 +2886,17 @@
         <v>7</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="H16" s="14" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2901,25 +2904,25 @@
         <v>9</v>
       </c>
       <c r="B17" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="F17" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="H17" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="I17" s="0" t="s">
         <v>133</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2927,17 +2930,17 @@
         <v>10</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="H18" s="0" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2945,25 +2948,25 @@
         <v>11</v>
       </c>
       <c r="B19" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="E19" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="F19" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="H19" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>144</v>
-      </c>
       <c r="I19" s="0" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2971,23 +2974,23 @@
         <v>12</v>
       </c>
       <c r="B20" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E20" s="12" t="s">
         <v>145</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>148</v>
       </c>
       <c r="F20" s="12"/>
       <c r="H20" s="0" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2995,23 +2998,23 @@
         <v>13</v>
       </c>
       <c r="B21" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="E21" s="12" t="s">
         <v>150</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>153</v>
       </c>
       <c r="F21" s="12"/>
       <c r="H21" s="0" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3019,23 +3022,23 @@
         <v>14</v>
       </c>
       <c r="B22" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>155</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>158</v>
       </c>
       <c r="F22" s="12"/>
       <c r="H22" s="0" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3043,20 +3046,20 @@
         <v>15</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="H23" s="12" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3064,19 +3067,19 @@
         <v>16</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
       <c r="H24" s="0" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3084,25 +3087,25 @@
         <v>17</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
       <c r="H25" s="0" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="19"/>
       <c r="B26" s="14" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
@@ -3118,12 +3121,12 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3145,7 +3148,7 @@
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="19"/>
       <c r="B32" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
@@ -3157,10 +3160,10 @@
         <v>1</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
@@ -3171,10 +3174,10 @@
         <v>2</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
@@ -3185,10 +3188,10 @@
         <v>3</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
@@ -3199,10 +3202,10 @@
         <v>4</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
@@ -3213,10 +3216,10 @@
         <v>5</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
@@ -3249,7 +3252,7 @@
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="19"/>
       <c r="B41" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
@@ -3261,10 +3264,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
@@ -3275,10 +3278,10 @@
         <v>2</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
@@ -3289,10 +3292,10 @@
         <v>3</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
@@ -3303,7 +3306,7 @@
         <v>4</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
@@ -3332,7 +3335,7 @@
       <selection pane="topLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="4.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.67"/>
@@ -3352,52 +3355,52 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="20" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="18" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="18" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="12" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -3405,7 +3408,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="12" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
@@ -3413,220 +3416,220 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="21" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C16" s="21"/>
       <c r="E16" s="21" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F16" s="21"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="22" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C17" s="23"/>
       <c r="E17" s="24" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F17" s="23"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="22" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C18" s="23"/>
       <c r="E18" s="24" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F18" s="23"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="22" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C19" s="23"/>
       <c r="E19" s="24" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F19" s="23"/>
     </row>
     <row r="20" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="22" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C20" s="23"/>
       <c r="E20" s="24" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F20" s="23"/>
     </row>
     <row r="21" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="22" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C21" s="23"/>
       <c r="E21" s="24" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F21" s="23"/>
     </row>
     <row r="22" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="22" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C22" s="23"/>
       <c r="E22" s="24" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F22" s="23"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="22" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C23" s="23"/>
       <c r="E23" s="24" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F23" s="23"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="22" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C24" s="23"/>
       <c r="E24" s="24" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F24" s="23"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="22" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C25" s="23"/>
       <c r="E25" s="24" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F25" s="23"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="25" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C26" s="26"/>
       <c r="E26" s="27" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F26" s="26"/>
     </row>
     <row r="28" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="21" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C28" s="21"/>
       <c r="E28" s="28" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F28" s="28"/>
     </row>
     <row r="29" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="22" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C29" s="23"/>
       <c r="E29" s="24" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F29" s="23"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="22" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C30" s="23"/>
       <c r="E30" s="24" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F30" s="23"/>
     </row>
     <row r="31" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="22" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C31" s="23"/>
       <c r="E31" s="24" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F31" s="23"/>
     </row>
     <row r="32" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="22" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C32" s="23"/>
       <c r="E32" s="24" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F32" s="23"/>
     </row>
     <row r="33" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="22" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C33" s="23"/>
       <c r="E33" s="24" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F33" s="23"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="22" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C34" s="23"/>
       <c r="E34" s="24" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F34" s="23"/>
     </row>
     <row r="35" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="22" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C35" s="23"/>
       <c r="E35" s="27" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F35" s="26"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="22" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C36" s="23"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="22" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C37" s="23"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="25" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C38" s="26"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="61.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3647,7 +3650,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
@@ -3659,7 +3662,7 @@
         <v>1</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3667,7 +3670,7 @@
         <v>2</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3675,7 +3678,7 @@
         <v>3</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3683,7 +3686,7 @@
         <v>4</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3691,42 +3694,42 @@
         <v>5</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="29" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B65" s="30" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C65" s="30"/>
       <c r="D65" s="30"/>
@@ -3735,7 +3738,7 @@
     </row>
     <row r="68" customFormat="false" ht="84" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B68" s="30" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C68" s="30"/>
       <c r="D68" s="30"/>
@@ -3744,12 +3747,12 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C72" s="14"/>
     </row>
@@ -3761,10 +3764,10 @@
         <v>1</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3772,10 +3775,10 @@
         <v>2</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3783,13 +3786,13 @@
         <v>3</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3797,20 +3800,20 @@
         <v>4</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B78" s="31" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C78" s="31"/>
       <c r="D78" s="31"/>
       <c r="E78" s="0" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3870,25 +3873,25 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="0" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="56" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B96" s="30" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C96" s="30"/>
       <c r="D96" s="30"/>
@@ -3926,7 +3929,7 @@
       <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.5"/>
@@ -3938,7 +3941,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3946,7 +3949,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3954,10 +3957,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3965,10 +3968,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3976,10 +3979,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3987,7 +3990,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3995,7 +3998,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4003,7 +4006,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4011,10 +4014,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4022,10 +4025,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4033,10 +4036,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4044,7 +4047,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4052,7 +4055,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4060,10 +4063,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4074,7 +4077,7 @@
     </row>
     <row r="17" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="32" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4082,17 +4085,17 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="33" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
@@ -4100,30 +4103,30 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="F24" s="23" t="s">
         <v>285</v>
-      </c>
-      <c r="D24" s="34" t="s">
-        <v>286</v>
-      </c>
-      <c r="E24" s="34" t="s">
-        <v>287</v>
-      </c>
-      <c r="F24" s="23" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="22" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E25" s="34" t="n">
         <v>1000</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4146,12 +4149,12 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="33" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D32" s="33"/>
       <c r="E32" s="33"/>
@@ -4159,27 +4162,27 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="22" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E33" s="34"/>
       <c r="F33" s="23"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="22" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E34" s="34"/>
       <c r="F34" s="23"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="22" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D35" s="34" t="n">
         <v>1000</v>
@@ -4189,30 +4192,30 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="D36" s="34" t="s">
         <v>288</v>
-      </c>
-      <c r="D36" s="34" t="s">
-        <v>291</v>
       </c>
       <c r="E36" s="34"/>
       <c r="F36" s="23"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="22" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D37" s="34" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E37" s="34"/>
       <c r="F37" s="23"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="22" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D38" s="34" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E38" s="34"/>
       <c r="F38" s="23"/>
@@ -4225,30 +4228,30 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="25" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D40" s="35"/>
       <c r="E40" s="35"/>
       <c r="F40" s="26" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="0" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="7" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -4278,7 +4281,7 @@
       <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="10.67"/>
@@ -4292,42 +4295,42 @@
   <sheetData>
     <row r="2" customFormat="false" ht="25.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>301</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>303</v>
-      </c>
-      <c r="I2" s="36" t="s">
-        <v>304</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>307</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>308</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="G3" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>309</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="L3" s="0" t="s">
         <v>310</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>311</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>305</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4335,13 +4338,13 @@
         <v>1</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4349,10 +4352,10 @@
         <v>2</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4360,7 +4363,7 @@
         <v>3</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4370,114 +4373,114 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J8" s="7" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J9" s="0" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J10" s="0" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J11" s="0" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J12" s="0" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J13" s="0" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J20" s="0" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J21" s="0" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="7" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="17" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -4489,7 +4492,7 @@
     </row>
     <row r="27" customFormat="false" ht="25.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="17" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -4501,7 +4504,7 @@
     </row>
     <row r="28" customFormat="false" ht="25.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="17" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -4513,7 +4516,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="17" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -4525,7 +4528,7 @@
     </row>
     <row r="30" customFormat="false" ht="25.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="17" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>

</xml_diff>